<commit_message>
Updating BOM for mirrored STL
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="115">
   <si>
     <t>PART NUMBER</t>
   </si>
@@ -315,6 +315,9 @@
   </si>
   <si>
     <t>FRAME VERTEX WITH FOOT</t>
+  </si>
+  <si>
+    <t>FRAME VERTEX WITH FOOT(MIRRORED)</t>
   </si>
   <si>
     <t>FRAME VERTEX WITHOUT FOOT</t>
@@ -454,10 +457,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E98"/>
+  <dimension ref="A1:E99"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A86" activeCellId="0" sqref="A86"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A55" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C87" activeCellId="0" sqref="C87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1914,7 +1917,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="n">
         <v>910</v>
       </c>
@@ -1928,12 +1931,12 @@
         <v>92</v>
       </c>
       <c r="E86" s="0" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="n">
-        <v>912</v>
+        <v>1010</v>
       </c>
       <c r="B87" s="0" t="s">
         <v>5</v>
@@ -1950,7 +1953,7 @@
     </row>
     <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="n">
-        <v>914</v>
+        <v>912</v>
       </c>
       <c r="B88" s="0" t="s">
         <v>5</v>
@@ -1962,15 +1965,15 @@
         <v>92</v>
       </c>
       <c r="E88" s="0" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="n">
-        <v>916</v>
+        <v>914</v>
       </c>
       <c r="B89" s="0" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C89" s="0" t="s">
         <v>102</v>
@@ -1979,15 +1982,15 @@
         <v>92</v>
       </c>
       <c r="E89" s="0" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="n">
-        <v>917</v>
+        <v>916</v>
       </c>
       <c r="B90" s="0" t="s">
-        <v>96</v>
+        <v>8</v>
       </c>
       <c r="C90" s="0" t="s">
         <v>103</v>
@@ -2001,10 +2004,10 @@
     </row>
     <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="0" t="n">
-        <v>935</v>
+        <v>917</v>
       </c>
       <c r="B91" s="0" t="s">
-        <v>5</v>
+        <v>96</v>
       </c>
       <c r="C91" s="0" t="s">
         <v>104</v>
@@ -2018,7 +2021,7 @@
     </row>
     <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="0" t="n">
-        <v>939</v>
+        <v>935</v>
       </c>
       <c r="B92" s="0" t="s">
         <v>5</v>
@@ -2030,12 +2033,12 @@
         <v>92</v>
       </c>
       <c r="E92" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="0" t="n">
-        <v>940</v>
+        <v>939</v>
       </c>
       <c r="B93" s="0" t="s">
         <v>5</v>
@@ -2047,12 +2050,12 @@
         <v>92</v>
       </c>
       <c r="E93" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="0" t="n">
-        <v>945</v>
+        <v>940</v>
       </c>
       <c r="B94" s="0" t="s">
         <v>5</v>
@@ -2069,7 +2072,7 @@
     </row>
     <row r="95" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="0" t="n">
-        <v>947</v>
+        <v>945</v>
       </c>
       <c r="B95" s="0" t="s">
         <v>5</v>
@@ -2086,7 +2089,7 @@
     </row>
     <row r="96" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="0" t="n">
-        <v>948</v>
+        <v>947</v>
       </c>
       <c r="B96" s="0" t="s">
         <v>5</v>
@@ -2103,7 +2106,7 @@
     </row>
     <row r="97" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="0" t="n">
-        <v>949</v>
+        <v>948</v>
       </c>
       <c r="B97" s="0" t="s">
         <v>5</v>
@@ -2120,18 +2123,35 @@
     </row>
     <row r="98" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="0" t="n">
+        <v>949</v>
+      </c>
+      <c r="B98" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C98" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="D98" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="E98" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="99" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A99" s="0" t="n">
         <v>579</v>
       </c>
-      <c r="B98" s="0" t="s">
-        <v>111</v>
-      </c>
-      <c r="C98" s="0" t="s">
+      <c r="B99" s="0" t="s">
         <v>112</v>
       </c>
-      <c r="D98" s="0" t="s">
+      <c r="C99" s="0" t="s">
         <v>113</v>
       </c>
-      <c r="E98" s="0" t="n">
+      <c r="D99" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="E99" s="0" t="n">
         <v>4</v>
       </c>
     </row>

</xml_diff>